<commit_message>
Small additions and final test
Added client 3 as test.
Publish summary report to allocated folder.
</commit_message>
<xml_diff>
--- a/Client 2/Disability.xlsx
+++ b/Client 2/Disability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolph Van Rensburg\Desktop\KHUSA\Clarissa Summary Report\Client 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC6C409-9A13-41E4-BE1B-EBD3112995B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53E4D0E-D03E-4BB5-A96C-619736D9AF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-96" windowWidth="29016" windowHeight="16416" xr2:uid="{C1AA6538-AF1B-44EF-AEDD-64799C5F45FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C1AA6538-AF1B-44EF-AEDD-64799C5F45FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Disabilities" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <t>Member C</t>
   </si>
   <si>
-    <t>Member E</t>
+    <t>Member D</t>
   </si>
 </sst>
 </file>
@@ -923,7 +923,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,14 +1064,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d023f3b7-3b52-4817-a6b9-85ddf5945990" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c7dd1ac-56d3-4e98-9913-357e1eb00778">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1336,21 +1334,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d023f3b7-3b52-4817-a6b9-85ddf5945990" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c7dd1ac-56d3-4e98-9913-357e1eb00778">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FF65F3C-ADAE-41E9-8C0C-C9E8CF498628}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E7A88F8-EB3B-4287-A0F2-7819DD2EF5A0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d023f3b7-3b52-4817-a6b9-85ddf5945990"/>
-    <ds:schemaRef ds:uri="7c7dd1ac-56d3-4e98-9913-357e1eb00778"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1375,9 +1372,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E7A88F8-EB3B-4287-A0F2-7819DD2EF5A0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FF65F3C-ADAE-41E9-8C0C-C9E8CF498628}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d023f3b7-3b52-4817-a6b9-85ddf5945990"/>
+    <ds:schemaRef ds:uri="7c7dd1ac-56d3-4e98-9913-357e1eb00778"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>